<commit_message>
journal merge dans le main
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Andrei-PiresDonose.xlsx
+++ b/documentation/3_1_Journal-Andrei-PiresDonose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-G1-Piloter_un_robot_phidget_a_distance\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60C79DE0-D8FD-46D6-B27B-A4FB38D90D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072C55FA-6A0C-4EF9-A41C-25279731AD24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3915" yWindow="1530" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal_NOM_PRENOM" sheetId="8" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -101,6 +101,22 @@
   </si>
   <si>
     <t>J'ai passé toute l'après midi à faire un bon business Case pour avoir une grande notion de quoi va parler notre projet pour qu'on le puisse ensuite le dévélopper.</t>
+  </si>
+  <si>
+    <t>Fait la connexion entre le phidget et le PC hôte</t>
+  </si>
+  <si>
+    <t>Renseignement sur les moyens de connectivité entre le serveur phidget et le frontend</t>
+  </si>
+  <si>
+    <t>Fait le site web pour afficher les informations du robot minimalistes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fait le manuel d'utilisateur </t>
+  </si>
+  <si>
+    <t>Dans la matinée, j’ai commencé par connecter le Phidget au PC hôte et vérifier que la communication fonctionnait bien. Ensuite, je me suis renseigné sur les différentes méthodes de connectivité entre le serveur Phidget et le frontend, afin de comprendre comment transmettre efficacement les données au site web.
+Dans l' après-midi, j’ai créé un site web minimaliste pour afficher les informations du robot, avec une interface simple et claire. Pour finir, j’ai rédigé le manuel d’utilisateur, expliquant l’installation, la connexion au Phidget et l’utilisation du site. J'ai trouvé que ça allait bien mais on faisait pas correctement le Kanban et la documentation. J'ai été très focus à mon code et l'expérimentation</t>
   </si>
 </sst>
 </file>
@@ -397,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -446,6 +462,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -482,6 +502,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -494,59 +518,85 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1177,7 +1227,7 @@
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
       <pane ySplit="1" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="B12" sqref="B12:D12"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1228,7 +1278,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="A6" s="36">
         <v>45996</v>
       </c>
       <c r="B6" s="32" t="s">
@@ -1240,31 +1290,31 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="18"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1277,45 +1327,63 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="14">
+        <v>46003</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="38"/>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="8"/>
+      <c r="A14" s="15"/>
+      <c r="B14" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="8">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="8"/>
+      <c r="A15" s="15"/>
+      <c r="B15" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="40"/>
+      <c r="D15" s="8">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="8"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1324,47 +1392,49 @@
       </c>
       <c r="D18" s="9">
         <f>SUM(D13:D17)</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="21"/>
+      <c r="D19" s="22"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="16"/>
+      <c r="C20" s="17"/>
       <c r="D20" s="7"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1377,43 +1447,43 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
+      <c r="A27" s="14"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="19"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1426,43 +1496,43 @@
       </c>
     </row>
     <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="25"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="26"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="19"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="19"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="19"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="19"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1475,43 +1545,43 @@
       </c>
     </row>
     <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="25"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="A40" s="23"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="26"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="16"/>
+      <c r="C41" s="17"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="19"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="19"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1524,43 +1594,43 @@
       </c>
     </row>
     <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="25"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="24"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="26"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="17"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="18"/>
+      <c r="C49" s="19"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="18"/>
+      <c r="C50" s="19"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="18"/>
+      <c r="C51" s="19"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="18"/>
+      <c r="C52" s="19"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1573,43 +1643,43 @@
       </c>
     </row>
     <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="25"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
+      <c r="A54" s="23"/>
+      <c r="B54" s="24"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="26"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="16"/>
+      <c r="C55" s="17"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="18"/>
+      <c r="C57" s="19"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="18"/>
+      <c r="C58" s="19"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="19"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1622,43 +1692,43 @@
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="25"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
+      <c r="A61" s="23"/>
+      <c r="B61" s="24"/>
+      <c r="C61" s="25"/>
+      <c r="D61" s="26"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="17"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="19"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="18"/>
+      <c r="C64" s="19"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="18"/>
+      <c r="C65" s="19"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="18"/>
+      <c r="C66" s="19"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1671,43 +1741,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="20"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="22"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="16"/>
+      <c r="C69" s="17"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="18"/>
+      <c r="C70" s="19"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="18"/>
+      <c r="C71" s="19"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="18"/>
+      <c r="C72" s="19"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="18"/>
+      <c r="C73" s="19"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1720,43 +1790,43 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="25"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
+      <c r="A75" s="23"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="25"/>
+      <c r="D75" s="26"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="16"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="16"/>
+      <c r="C76" s="17"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="18"/>
+      <c r="C77" s="19"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="18"/>
+      <c r="C78" s="19"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="19"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="19"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1769,10 +1839,10 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="25"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="24"/>
+      <c r="A82" s="23"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="25"/>
+      <c r="D82" s="26"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1782,19 +1852,85 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>3.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="36" t="s">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="B13:C13"/>
@@ -1811,167 +1947,101 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D6)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13:D18">
-    <cfRule type="containsText" dxfId="21" priority="21" operator="containsText" text="Terminé">
-      <formula>NOT(ISERROR(SEARCH("Terminé",D13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="22" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="D20:D25">
-    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="21" priority="5" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="4" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="20" priority="6" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D27:D32">
-    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="19" priority="21" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D27)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D34:D39">
-    <cfRule type="containsText" dxfId="15" priority="17" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="17" priority="19" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D34)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="18" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D34)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D41:D46">
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="15" priority="11" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D41)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D41)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D48:D53">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D48)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="12" priority="10" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D55:D60">
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D55)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D62:D67">
-    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="9" priority="17" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D62)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="8" priority="18" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D69:D74">
-    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="7" priority="15" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D69)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="6" priority="16" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D76:D81">
-    <cfRule type="containsText" dxfId="3" priority="11" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D76)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="12" operator="containsText" text="En cours">
+    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="En cours">
       <formula>NOT(ISERROR(SEARCH("En cours",D76)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D83">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Terminé">
       <formula>NOT(ISERROR(SEARCH("Terminé",D83)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="En cours">
+      <formula>NOT(ISERROR(SEARCH("En cours",D83)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13:D18">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Terminé">
+      <formula>NOT(ISERROR(SEARCH("Terminé",D13)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="En cours">
-      <formula>NOT(ISERROR(SEARCH("En cours",D83)))</formula>
+      <formula>NOT(ISERROR(SEARCH("En cours",D13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions horizontalCentered="1"/>
@@ -1991,6 +2061,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
@@ -1999,15 +2078,6 @@
     <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2224,6 +2294,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2232,14 +2310,6 @@
     <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
     <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
     <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
psuh journal et doc
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Andrei-PiresDonose.xlsx
+++ b/documentation/3_1_Journal-Andrei-PiresDonose.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-G1-Piloter_un_robot_phidget_a_distance\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3359523-F4E7-4E42-9E5B-A28C30235E55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27170443-057E-42C9-B160-D08108B35838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="20220" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Journal_NOM_PRENOM" sheetId="8" r:id="rId1"/>
+    <sheet name="Journal_PIRESDONOSE_ANDREI" sheetId="8" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal_NOM_PRENOM!$A$5:$HI$5</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal_NOM_PRENOM!$B:$D,Journal_NOM_PRENOM!$1:$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_NOM_PRENOM!$A$1:$D$83</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Journal_PIRESDONOSE_ANDREI!$A$5:$HI$5</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Journal_PIRESDONOSE_ANDREI!$B:$D,Journal_PIRESDONOSE_ANDREI!$1:$5</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal_PIRESDONOSE_ANDREI!$A$1:$D$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -117,6 +117,18 @@
   <si>
     <t>Dans la matinée, j’ai commencé par connecter le Phidget au PC hôte et vérifier que la communication fonctionnait bien. Ensuite, je me suis renseigné sur les différentes méthodes de connectivité entre le serveur Phidget et le frontend, afin de comprendre comment transmettre efficacement les données au site web.
 Dans l' après-midi, j’ai créé un site web minimaliste pour afficher les informations du robot, avec une interface simple et claire. Pour finir, j’ai rédigé le manuel d’utilisateur, expliquant l’installation, la connexion au Phidget et l’utilisation du site. J'ai trouvé que ça allait bien mais on faisait pas correctement le Kanban et la documentation. J'ai été très focus à mon code et l'expérimentation.</t>
+  </si>
+  <si>
+    <t>Fait la Definition of Done"</t>
+  </si>
+  <si>
+    <t>Fait la structure du projet avec les bons dossiers</t>
+  </si>
+  <si>
+    <t>Aider à la compréhension du problème de connexion sans fil de la manette</t>
+  </si>
+  <si>
+    <t>Dans la journée, j’ai travaillé sur la Definition of Done pour mieux comprendre à quel moment une tâche peut être considérée comme terminée. J’ai ensuite mis en place une structure de projet avec les bons dossiers pour améliorer l’organisation. J’ai également  aidé à mieux comprendre le problème de connexion sans fil lié à la manette. J’ai constaté que je me suis amélioré dans l’utilisation de la méthode agile, surtout en documentant davantage chaque étape et en utilisant mieux le Kanban.</t>
   </si>
 </sst>
 </file>
@@ -462,6 +474,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -470,6 +486,42 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -478,26 +530,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -510,65 +542,45 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1203,9 +1215,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19:D19"/>
+      <selection pane="bottomLeft" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1218,81 +1230,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="A6" s="40">
         <v>45996</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7">
         <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1305,63 +1317,63 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+      <c r="A13" s="14">
         <v>46003</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="39" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1374,45 +1386,59 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="7"/>
+      <c r="A20" s="14">
+        <v>46009</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="7">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="18"/>
-      <c r="D21" s="8"/>
+      <c r="A21" s="15"/>
+      <c r="B21" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="21"/>
+      <c r="D21" s="8">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="8"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1421,47 +1447,51 @@
       </c>
       <c r="D25" s="9">
         <f>SUM(D20:D24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="15"/>
+      <c r="B26" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="16"/>
+      <c r="A27" s="14">
+        <v>46010</v>
+      </c>
+      <c r="B27" s="26"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="7"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="18"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1475,42 +1505,42 @@
     </row>
     <row r="33" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="16"/>
+      <c r="A34" s="14"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="7"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17"/>
-      <c r="C35" s="18"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1524,42 +1554,42 @@
     </row>
     <row r="40" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="25"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="16"/>
+      <c r="A41" s="14"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="7"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
+      <c r="A42" s="15"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="8"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="18"/>
+      <c r="A43" s="15"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1573,42 +1603,42 @@
     </row>
     <row r="47" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="25"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
+      <c r="A48" s="14"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="7"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1622,42 +1652,42 @@
     </row>
     <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="25"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="29"/>
+      <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
+      <c r="A55" s="14"/>
+      <c r="B55" s="26"/>
+      <c r="C55" s="27"/>
       <c r="D55" s="7"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="21"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="21"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1671,42 +1701,42 @@
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="30"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="21"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="21"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="21"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1719,43 +1749,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="24"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="21"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="21"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="21"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1769,42 +1799,42 @@
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="25"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="30"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="16"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="21"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="21"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="21"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="21"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1818,9 +1848,9 @@
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="25"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="24"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="30"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1830,19 +1860,85 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>10.5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="36" t="s">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="B13:C13"/>
@@ -1859,72 +1955,6 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Terminé">
@@ -2048,6 +2078,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2260,17 +2301,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
@@ -2280,6 +2310,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2296,17 +2339,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update documentation plus journal Andrei
</commit_message>
<xml_diff>
--- a/documentation/3_1_Journal-Andrei-PiresDonose.xlsx
+++ b/documentation/3_1_Journal-Andrei-PiresDonose.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\306-G1-Piloter_un_robot_phidget_a_distance\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F9116AB-5FB1-40EF-9CDC-E307261C1A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A54D216-45D3-4FEF-A40F-C3E215FA1435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
   <si>
     <t>Insérer les lignes au-dessus de celle-ci !</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Ce matin, j’ai commencé par développer la page du dashboard pour que l'utilisateur puisse se connecter au backend, puis vers le réseau Phidget. Dans l’après-midi, j’ai poursuivi la documentation sur les protocoles de test de chaque page. J'ai aussi réorganisé le frontend en changeant les noms et les dossiers pour garder une bonne structure. Globalement, j’ai trouvé que ça s'est bien passé aujourd'hui.</t>
+  </si>
+  <si>
+    <t>Aujourd'hui, j'ai finalisé les protocoles de test. J'ai pris le temps d'optimiser la structure pour éliminer les redondances et simplifier la lecture. Le résultat est désormais plus condensé et efficace. Globalement, la journée a été productive.</t>
+  </si>
+  <si>
+    <t>Tester l'application avec Luuk</t>
   </si>
 </sst>
 </file>
@@ -506,6 +512,10 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -514,6 +524,42 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
@@ -522,26 +568,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -554,65 +580,45 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1247,9 +1253,9 @@
   <dimension ref="A1:D84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft"/>
       <selection activeCell="D5" sqref="A5:XFD5"/>
-      <selection pane="bottomLeft" activeCell="H46" sqref="H46"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1262,81 +1268,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34"/>
-      <c r="C2" s="35"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="39"/>
       <c r="D2" s="4">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="29"/>
+      <c r="C4" s="33"/>
       <c r="D4" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="35"/>
       <c r="D5" s="6" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="26">
+      <c r="A6" s="40">
         <v>45996</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="33"/>
+      <c r="C6" s="37"/>
       <c r="D6" s="7">
         <v>3.5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
+      <c r="A7" s="15"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="21"/>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
+      <c r="A9" s="15"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="21"/>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
+      <c r="A10" s="15"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="21"/>
       <c r="D10" s="8"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="14"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1349,63 +1355,63 @@
       </c>
     </row>
     <row r="12" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="15"/>
+      <c r="B12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="21"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="24"/>
     </row>
     <row r="13" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13">
+      <c r="A13" s="14">
         <v>46003</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="17"/>
       <c r="D13" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="39" t="s">
+      <c r="A14" s="15"/>
+      <c r="B14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="40"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="40"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="8">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
-      <c r="B16" s="39" t="s">
+      <c r="A16" s="15"/>
+      <c r="B16" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="40"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="14"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="21"/>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="2" t="s">
         <v>6</v>
       </c>
@@ -1418,59 +1424,59 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="87.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
-      <c r="B19" s="19" t="s">
+      <c r="A19" s="15"/>
+      <c r="B19" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="21"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="24"/>
     </row>
     <row r="20" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13">
+      <c r="A20" s="14">
         <v>46009</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="16"/>
+      <c r="C20" s="27"/>
       <c r="D20" s="7">
         <v>1.5</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="15"/>
+      <c r="B21" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="18"/>
+      <c r="C21" s="21"/>
       <c r="D21" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="17" t="s">
+      <c r="A22" s="15"/>
+      <c r="B22" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="18"/>
+      <c r="C22" s="21"/>
       <c r="D22" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="14"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1483,55 +1489,55 @@
       </c>
     </row>
     <row r="26" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
-      <c r="B26" s="19" t="s">
+      <c r="A26" s="15"/>
+      <c r="B26" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="24"/>
     </row>
     <row r="27" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>46010</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="16"/>
+      <c r="C27" s="27"/>
       <c r="D27" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="15"/>
+      <c r="B28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="18"/>
+      <c r="C28" s="21"/>
       <c r="D28" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="14"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="18"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="21"/>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="18"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="21"/>
       <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="18"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="21"/>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="2" t="s">
         <v>6</v>
       </c>
@@ -1545,54 +1551,54 @@
     </row>
     <row r="33" spans="1:4" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="25"/>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="23"/>
-      <c r="D33" s="24"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
     </row>
     <row r="34" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+      <c r="A34" s="14">
         <v>46030</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C34" s="16"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="7">
         <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="14"/>
-      <c r="B35" s="17" t="s">
+      <c r="A35" s="15"/>
+      <c r="B35" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C35" s="18"/>
+      <c r="C35" s="21"/>
       <c r="D35" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
-      <c r="B36" s="17"/>
-      <c r="C36" s="18"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="21"/>
       <c r="D36" s="8"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
-      <c r="B37" s="17"/>
-      <c r="C37" s="18"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="21"/>
       <c r="D37" s="8"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18"/>
+      <c r="A38" s="15"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
       <c r="D38" s="8"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="2" t="s">
         <v>6</v>
       </c>
@@ -1606,58 +1612,58 @@
     </row>
     <row r="40" spans="1:4" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="25"/>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="C40" s="23"/>
-      <c r="D40" s="24"/>
+      <c r="C40" s="29"/>
+      <c r="D40" s="30"/>
     </row>
     <row r="41" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13">
+      <c r="A41" s="14">
         <v>46031</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C41" s="16"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="7">
         <v>3.5</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
-      <c r="B42" s="17" t="s">
+      <c r="A42" s="15"/>
+      <c r="B42" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="18"/>
+      <c r="C42" s="21"/>
       <c r="D42" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
-      <c r="B43" s="17" t="s">
+      <c r="A43" s="15"/>
+      <c r="B43" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C43" s="18"/>
+      <c r="C43" s="21"/>
       <c r="D43" s="8">
         <v>0.5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="18"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="20"/>
+      <c r="C44" s="21"/>
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="18"/>
+      <c r="A45" s="15"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
       <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="2" t="s">
         <v>6</v>
       </c>
@@ -1671,44 +1677,50 @@
     </row>
     <row r="47" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="25"/>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C47" s="23"/>
-      <c r="D47" s="24"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="30"/>
     </row>
     <row r="48" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="7"/>
+      <c r="A48" s="14">
+        <v>46037</v>
+      </c>
+      <c r="B48" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="27"/>
+      <c r="D48" s="7">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="14"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18"/>
+      <c r="A49" s="15"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
       <c r="D49" s="8"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="14"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18"/>
+      <c r="A50" s="15"/>
+      <c r="B50" s="20"/>
+      <c r="C50" s="21"/>
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="14"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="18"/>
+      <c r="A51" s="15"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
       <c r="D51" s="8"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" s="14"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="18"/>
+      <c r="A52" s="15"/>
+      <c r="B52" s="20"/>
+      <c r="C52" s="21"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A53" s="14"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="2" t="s">
         <v>6</v>
       </c>
@@ -1717,47 +1729,57 @@
       </c>
       <c r="D53" s="9">
         <f>SUM(D48:D52)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="25"/>
-      <c r="B54" s="22"/>
-      <c r="C54" s="23"/>
-      <c r="D54" s="24"/>
+      <c r="B54" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" s="29"/>
+      <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="7"/>
+      <c r="A55" s="14">
+        <v>46038</v>
+      </c>
+      <c r="B55" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="7">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A56" s="14"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="18"/>
-      <c r="D56" s="8"/>
+      <c r="A56" s="15"/>
+      <c r="B56" s="20"/>
+      <c r="C56" s="21"/>
+      <c r="D56" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A57" s="14"/>
-      <c r="B57" s="17"/>
-      <c r="C57" s="18"/>
+      <c r="A57" s="15"/>
+      <c r="B57" s="20"/>
+      <c r="C57" s="21"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="14"/>
-      <c r="B58" s="17"/>
-      <c r="C58" s="18"/>
+      <c r="A58" s="15"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="21"/>
       <c r="D58" s="8"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="17"/>
-      <c r="C59" s="18"/>
+      <c r="A59" s="15"/>
+      <c r="B59" s="20"/>
+      <c r="C59" s="21"/>
       <c r="D59" s="8"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A60" s="14"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="2" t="s">
         <v>6</v>
       </c>
@@ -1766,47 +1788,47 @@
       </c>
       <c r="D60" s="9">
         <f>SUM(D55:D59)</f>
-        <v>0</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="25"/>
-      <c r="B61" s="22"/>
-      <c r="C61" s="23"/>
-      <c r="D61" s="24"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="29"/>
+      <c r="D61" s="30"/>
     </row>
     <row r="62" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="16"/>
+      <c r="A62" s="14"/>
+      <c r="B62" s="26"/>
+      <c r="C62" s="27"/>
       <c r="D62" s="7"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="17"/>
-      <c r="C63" s="18"/>
+      <c r="A63" s="15"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="21"/>
       <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="17"/>
-      <c r="C64" s="18"/>
+      <c r="A64" s="15"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="21"/>
       <c r="D64" s="8"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="14"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="18"/>
+      <c r="A65" s="15"/>
+      <c r="B65" s="20"/>
+      <c r="C65" s="21"/>
       <c r="D65" s="8"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="14"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="18"/>
+      <c r="A66" s="15"/>
+      <c r="B66" s="20"/>
+      <c r="C66" s="21"/>
       <c r="D66" s="8"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="14"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="2" t="s">
         <v>6</v>
       </c>
@@ -1819,43 +1841,43 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="14"/>
-      <c r="B68" s="19"/>
-      <c r="C68" s="20"/>
-      <c r="D68" s="21"/>
+      <c r="A68" s="15"/>
+      <c r="B68" s="22"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="24"/>
     </row>
     <row r="69" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13"/>
-      <c r="B69" s="15"/>
-      <c r="C69" s="16"/>
+      <c r="A69" s="14"/>
+      <c r="B69" s="26"/>
+      <c r="C69" s="27"/>
       <c r="D69" s="7"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="14"/>
-      <c r="B70" s="17"/>
-      <c r="C70" s="18"/>
+      <c r="A70" s="15"/>
+      <c r="B70" s="20"/>
+      <c r="C70" s="21"/>
       <c r="D70" s="8"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="14"/>
-      <c r="B71" s="17"/>
-      <c r="C71" s="18"/>
+      <c r="A71" s="15"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
       <c r="D71" s="8"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="14"/>
-      <c r="B72" s="17"/>
-      <c r="C72" s="18"/>
+      <c r="A72" s="15"/>
+      <c r="B72" s="20"/>
+      <c r="C72" s="21"/>
       <c r="D72" s="8"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="14"/>
-      <c r="B73" s="17"/>
-      <c r="C73" s="18"/>
+      <c r="A73" s="15"/>
+      <c r="B73" s="20"/>
+      <c r="C73" s="21"/>
       <c r="D73" s="8"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="14"/>
+      <c r="A74" s="15"/>
       <c r="B74" s="2" t="s">
         <v>6</v>
       </c>
@@ -1869,42 +1891,42 @@
     </row>
     <row r="75" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="25"/>
-      <c r="B75" s="22"/>
-      <c r="C75" s="23"/>
-      <c r="D75" s="24"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="29"/>
+      <c r="D75" s="30"/>
     </row>
     <row r="76" spans="1:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="15"/>
-      <c r="C76" s="16"/>
+      <c r="A76" s="14"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="27"/>
       <c r="D76" s="7"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="14"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="18"/>
+      <c r="A77" s="15"/>
+      <c r="B77" s="20"/>
+      <c r="C77" s="21"/>
       <c r="D77" s="8"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="14"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="18"/>
+      <c r="A78" s="15"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="21"/>
       <c r="D78" s="8"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="14"/>
-      <c r="B79" s="17"/>
-      <c r="C79" s="18"/>
+      <c r="A79" s="15"/>
+      <c r="B79" s="20"/>
+      <c r="C79" s="21"/>
       <c r="D79" s="8"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="14"/>
-      <c r="B80" s="17"/>
-      <c r="C80" s="18"/>
+      <c r="A80" s="15"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="21"/>
       <c r="D80" s="8"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="14"/>
+      <c r="A81" s="15"/>
       <c r="B81" s="2" t="s">
         <v>6</v>
       </c>
@@ -1918,9 +1940,9 @@
     </row>
     <row r="82" spans="1:4" ht="24.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="25"/>
-      <c r="B82" s="22"/>
-      <c r="C82" s="23"/>
-      <c r="D82" s="24"/>
+      <c r="B82" s="28"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="30"/>
     </row>
     <row r="83" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="11"/>
@@ -1930,19 +1952,85 @@
       </c>
       <c r="D83" s="12">
         <f>D11+D18+D25+D32+D39+D46+D53+D60+D67+D74+D81</f>
-        <v>31.5</v>
+        <v>38.5</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="36" t="s">
+      <c r="A84" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B84" s="36"/>
-      <c r="C84" s="36"/>
-      <c r="D84" s="36"/>
+      <c r="B84" s="13"/>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="82">
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:A61"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B61:D61"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="A76:A82"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:C78"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A69:A75"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B72:C72"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="A62:A68"/>
+    <mergeCell ref="B62:C62"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="A41:A47"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:A54"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="A6:A12"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B4:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A4:A5"/>
     <mergeCell ref="A84:D84"/>
     <mergeCell ref="A13:A19"/>
     <mergeCell ref="B13:C13"/>
@@ -1959,72 +2047,6 @@
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="B33:D33"/>
     <mergeCell ref="A34:A40"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="A6:A12"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="A62:A68"/>
-    <mergeCell ref="B62:C62"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="A41:A47"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:A54"/>
-    <mergeCell ref="A69:A75"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="B70:C70"/>
-    <mergeCell ref="B71:C71"/>
-    <mergeCell ref="B72:C72"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="A76:A82"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:C78"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:A61"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B61:D61"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B26:D26"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:D11">
     <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Terminé">
@@ -2148,6 +2170,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006BD0882D7B13D249A8B88997E24B9140" ma:contentTypeVersion="14" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="3865b25f2bf2a035dbe7787239b3f11c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8afaa137-8a18-4908-97f4-35fc924e5a91" xmlns:ns3="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="718f9f7ddd2530d56a17ab9424d0abda" ns2:_="" ns3:_="">
     <xsd:import namespace="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
@@ -2360,17 +2393,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8afaa137-8a18-4908-97f4-35fc924e5a91">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8C0AFF7-6D45-4588-A3CE-0506D82134A8}">
   <ds:schemaRefs>
@@ -2380,6 +2402,19 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
+    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
+    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
+    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{84AEF82B-2BAE-481D-A319-B09ADD6915E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2396,17 +2431,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1CED954-0C0B-4246-88BC-C0C5C061E08E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="b54f96d8-6138-4ba9-8b5a-da1062324abb"/>
-    <ds:schemaRef ds:uri="0ecde9c3-6951-4ee0-98d0-295e535ef6cd"/>
-    <ds:schemaRef ds:uri="8afaa137-8a18-4908-97f4-35fc924e5a91"/>
-    <ds:schemaRef ds:uri="3b60234b-33e6-42ae-ae88-ba7d4a3eedfd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>